<commit_message>
[framing] This [commit] solves the issues #1 and #2 that are labeled framing. 1. Removes all required fields except the mandatory fields defined by the stakeholder 2. Reframes the questions in evaluation form.
</commit_message>
<xml_diff>
--- a/app/src/utils/view-details.xlsx
+++ b/app/src/utils/view-details.xlsx
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,47 +418,55 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Full Name</v>
+        <v>ID</v>
       </c>
       <c r="B2" t="str">
-        <v>Frank Brano Gomes</v>
+        <v>66672ce348ccd80bebd64965</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Nick Name</v>
+        <v>Full Name</v>
       </c>
       <c r="B3" t="str">
-        <v>iamu985</v>
+        <v>Frank Brano Gomes</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Date of Birth</v>
+        <v>Nick Name</v>
       </c>
       <c r="B4" t="str">
-        <v>1999-01-01T00:00:00.000Z</v>
+        <v>iamu985</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Caste</v>
+        <v>Date of Birth</v>
       </c>
       <c r="B5" t="str">
-        <v>SC</v>
+        <v>1999-01-01T00:00:00.000Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>Caste</v>
+      </c>
+      <c r="B6" t="str">
+        <v>SC</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v>Religion</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B7" t="str">
         <v>Christian</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -715,10 +723,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ff</v>
+        <v>ffedited</v>
       </c>
       <c r="B2" t="str">
-        <v>mm</v>
+        <v>mm-edited</v>
       </c>
       <c r="C2" t="str">
         <v>ll</v>
@@ -751,7 +759,7 @@
         <v/>
       </c>
       <c r="M2" t="str">
-        <v>Yes</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>